<commit_message>
Hot fix: Míň děr v lokacích
</commit_message>
<xml_diff>
--- a/addresses.xlsx
+++ b/addresses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="159">
   <si>
     <t>ERASMUS CODE</t>
   </si>
@@ -22,316 +22,475 @@
     <t>Address</t>
   </si>
   <si>
+    <t>Univerzita</t>
+  </si>
+  <si>
     <t>BG ROUSSE01</t>
   </si>
   <si>
     <t>['STUDENTSKA STREET 8', 'RUSE', 'BG']</t>
   </si>
   <si>
+    <t xml:space="preserve">RUSENSKI UNIVERSITET ANGEL KUNCHEV  </t>
+  </si>
+  <si>
     <t>D  DORTMUN01</t>
   </si>
   <si>
     <t>['AUGUST SCHMIDT STRASSE 4', 'DORTMUND', 'DE']</t>
   </si>
   <si>
+    <t>Technische Universität Dortmund</t>
+  </si>
+  <si>
     <t>D  DRESDEN02</t>
   </si>
   <si>
     <t>['HELMHOLTZSTRASSE 10', 'DRESDEN', 'DE']</t>
   </si>
   <si>
+    <t xml:space="preserve">TECHNISCHE UNIVERSITÄT DRESDEN </t>
+  </si>
+  <si>
     <t>D  GIESSEN01</t>
   </si>
   <si>
     <t>['LUDWIGSTRASSE 23', 'GIESSEN', 'DE']</t>
   </si>
   <si>
+    <t xml:space="preserve">JUSTUS-LIEBIG-UNIVERSITÄT GIESSEN </t>
+  </si>
+  <si>
     <t>D  KAISERS01</t>
   </si>
   <si>
     <t>['GOTTLIEB DAIMLER STRASSE', 'KAISERSLAUTERN', 'DE']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERSITÄT KAISERSLAUTERN </t>
+  </si>
+  <si>
     <t>D  KOTHEN01</t>
   </si>
   <si>
     <t>['BERNBURGER STRASSE 55', 'KOETHEN', 'DE']</t>
   </si>
   <si>
+    <t>HOCHSCHULE ANHALT (FH)</t>
+  </si>
+  <si>
     <t>D  LEIPZIG01</t>
   </si>
   <si>
     <t>['RITTERSTRASSE  26', 'LEIPZIG', 'DE']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERSITÄT LEIPZIG </t>
+  </si>
+  <si>
     <t>D  ROSTOCK01</t>
   </si>
   <si>
     <t>['UNIVERSITATSPLATZ 1', 'ROSTOCK', 'DE']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERSITÄT ROSTOCK </t>
+  </si>
+  <si>
     <t>D  SIGMARI01</t>
   </si>
   <si>
     <t>['ANTON GUNTHER STRASSE 51', 'SIGMARINGEN', 'DE']</t>
   </si>
   <si>
+    <t>FACHHOCHSCHULE ALBSTADT-SIGMARINGEN</t>
+  </si>
+  <si>
     <t>D  WURZBUR01</t>
   </si>
   <si>
     <t>['SANDERRING  2', 'WUERZBURG', 'DE']</t>
   </si>
   <si>
+    <t>Julius-Maximilians Universität Würzburg</t>
+  </si>
+  <si>
     <t>E  JAEN01</t>
   </si>
   <si>
     <t>['CAMPUS LAS LAGUNILLAS SN EDIFICO B1 VICERRECTORADO DE INVESTIGACION DESAR TECN E INNOVACION', 'JAEN', 'ES']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERSIDAD DE JAÉN </t>
+  </si>
+  <si>
     <t>E  MADRID04</t>
   </si>
   <si>
     <t>['CALLE EINSTEIN 3 CIUDAD UNIV CANTOBLANCO RECTORADO', 'MADRID', 'ES']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERSIDAD AUTÓNOMA DE MADRID </t>
+  </si>
+  <si>
     <t>E  MALAGA01</t>
   </si>
   <si>
     <t>['AVDA CERVANTES, NUM. 2', 'MALAGA', 'ES']</t>
   </si>
   <si>
+    <t>UNIVERSIDAD DE MÁLAGA</t>
+  </si>
+  <si>
     <t>EE TALLINN05</t>
   </si>
   <si>
     <t>['Narva Road 25', 'TALLINN', 'EE']</t>
   </si>
   <si>
+    <t>Tallinna Ülikool</t>
+  </si>
+  <si>
     <t>F  ANGERS08</t>
   </si>
   <si>
     <t>['RUE RABELAIS 55', 'ANGERS CEDEX 1', 'FR']</t>
   </si>
   <si>
+    <t>ECOLE SUPERIEURE D'AGRICULTURE D'ANGERS</t>
+  </si>
+  <si>
     <t>F  TOULOUS15</t>
   </si>
   <si>
     <t>['VOIE DU TOEC 75', 'TOULOUSE', 'FR']</t>
   </si>
   <si>
+    <t>ECOLE SUPÉRIEURE D'AGRICULTURE DE PURPAN</t>
+  </si>
+  <si>
     <t>G  ATHINE41</t>
   </si>
   <si>
     <t>['LOFOS PANEPISTIMIOU', 'MYTILINI', 'EL']</t>
   </si>
   <si>
+    <t>PANEPISTIMIO EGEOU</t>
+  </si>
+  <si>
     <t>HR SPLIT01</t>
   </si>
   <si>
     <t>['RUDERA BOSKOVICA  31', 'SPLIT', 'HR']</t>
   </si>
   <si>
+    <t>SVEUCILISTE U SPLITU</t>
+  </si>
+  <si>
     <t>HR ZAGREB11</t>
   </si>
   <si>
     <t>['GRADISCANSKA 24', 'ZAGREB', 'HR']</t>
   </si>
   <si>
+    <t>ALGEBRA UNIVERSITY COLLEGE</t>
+  </si>
+  <si>
     <t>HU BUDAPES01</t>
   </si>
   <si>
     <t>['EGYETEM TER 1-3', 'BUDAPEST', 'HU']</t>
   </si>
   <si>
+    <t>EÖTVÖS LORÁND TUDOMÁNYEGYETEM</t>
+  </si>
+  <si>
     <t>I  CAMERIN01</t>
   </si>
   <si>
     <t>['PIAZZA CAVOUR 19F', 'CAMERINO', 'IT']</t>
   </si>
   <si>
+    <t>UNIVERSITA DEGLI STUDI DI CAMERINO</t>
+  </si>
+  <si>
     <t>I  TRIESTE01</t>
   </si>
   <si>
     <t>['PIAZZALE EUROPA 1', 'TRIESTE', 'IT']</t>
   </si>
   <si>
+    <t>UNIVERSITA DEGLI STUDI DI TRIESTE</t>
+  </si>
+  <si>
     <t>I  URBINO01</t>
   </si>
   <si>
     <t>['Via Aurelio Saffi  2', 'URBINO', 'IT']</t>
   </si>
   <si>
+    <t>UNIVERSITA DEGLI STUDI DI URBINO</t>
+  </si>
+  <si>
     <t>LT KAUNAS01</t>
   </si>
   <si>
     <t>['K DONELAICIO G 58', 'KAUNAS', 'LT']</t>
   </si>
   <si>
+    <t>VYTAUTO DIDZIOJO UNIVERSITETAS</t>
+  </si>
+  <si>
     <t>LV JELGAVA01</t>
   </si>
   <si>
     <t>['LIELA IELA 2', 'JELGAVA', 'LV']</t>
   </si>
   <si>
+    <t>LATVIJAS LAUKSAIMNIECÎBAS UNIVERSITÂTE</t>
+  </si>
+  <si>
     <t>P  LEIRIA01</t>
   </si>
   <si>
     <t>['Rua General Norton de Matos', 'Leiria', 'PT']</t>
   </si>
   <si>
+    <t>INSTITUTO POLITÉCNICO DE LEIRIA</t>
+  </si>
+  <si>
     <t>PL CZESTOC01</t>
   </si>
   <si>
     <t>['UL. DABROWSKIEGO 69', 'CZESTOCHOWA', 'PL']</t>
   </si>
   <si>
+    <t xml:space="preserve">POLITECHNIKA CZESTOCHOWSKA </t>
+  </si>
+  <si>
     <t>PL GDANSK01</t>
   </si>
   <si>
     <t>['UL. JANA BAZYNSKIEGO 8', 'GDANSK', 'PL']</t>
   </si>
   <si>
+    <t>UNIWERSYTET GDANSKI</t>
+  </si>
+  <si>
     <t>PL LODZ01</t>
   </si>
   <si>
     <t>['UL PREZYDENTA GABRIELA NARUTOWICZA 68', 'LODZ', 'PL']</t>
   </si>
   <si>
+    <t>UNIWERSYTET LÓDZKI</t>
+  </si>
+  <si>
     <t>PL LODZ02</t>
   </si>
   <si>
     <t>['ULICA ZEROMSKIEGO 116', 'LODZ', 'PL']</t>
   </si>
   <si>
+    <t>POLITECHNIKA LODZKA</t>
+  </si>
+  <si>
     <t>PL OPOLE01</t>
   </si>
   <si>
     <t>['PL MIKOLAJA KOPERNIKA 11A', 'OPOLE', 'PL']</t>
   </si>
   <si>
+    <t>UNIWERSYTET OPOLSKI</t>
+  </si>
+  <si>
     <t>PL POZNAN01</t>
   </si>
   <si>
     <t>['ULICA HENRYKA WIENIAWSKIEGO 1', 'POZNAN', 'PL']</t>
   </si>
   <si>
+    <t>Uniwersytet im. Adama Mickiewicza w Poznaniu</t>
+  </si>
+  <si>
     <t>PL SLUPSK01</t>
   </si>
   <si>
     <t>['UL KRZYSZTOFA ARCISZEWSKIEGO 22 A', 'SLUPSK', 'PL']</t>
   </si>
   <si>
+    <t>POMORSKA AKADEMIA PEDAGOGICZNA</t>
+  </si>
+  <si>
     <t>RO BUCURES09</t>
   </si>
   <si>
     <t>['SOSEAUA PANDURI 90', 'BUCURESTI', 'RO']</t>
   </si>
   <si>
+    <t>UNIVERSITATEA DIN BUCURESTI</t>
+  </si>
+  <si>
     <t>RO BUCURES18</t>
   </si>
   <si>
     <t>['BULEVARDUL EXPOZITIEI 1B SECTOR 1', 'BUCURESTI', 'RO']</t>
   </si>
   <si>
+    <t>UNIVERSITATEA ROMANO AMERICANA</t>
+  </si>
+  <si>
     <t>RO TIMISOA01</t>
   </si>
   <si>
     <t>['BD VASILE PARVAN 4', 'TIMISOARA', 'RO']</t>
   </si>
   <si>
+    <t>UNIVERSITATEA DE VEST DIN TIMISOARA</t>
+  </si>
+  <si>
     <t>RS NOVISAD02</t>
   </si>
   <si>
     <t>['DR ZORANA DINDICA 1', 'NOVI SAD', 'RS']</t>
   </si>
   <si>
+    <t>UNIVERZITET U NOVOM SADU</t>
+  </si>
+  <si>
     <t>S  UMEA01</t>
   </si>
   <si>
     <t>['UNIVERSITETOMRADET', 'UMEA', 'SE']</t>
   </si>
   <si>
+    <t>UMEA UNIVERSITET</t>
+  </si>
+  <si>
     <t>S  UPPSALA01</t>
   </si>
   <si>
     <t>['VON KRAEMERS ALLE 4', 'UPPSALA', 'SE']</t>
   </si>
   <si>
+    <t>UPPSALA UNIVERSITET</t>
+  </si>
+  <si>
     <t>SI KOPER03</t>
   </si>
   <si>
     <t>['TITOV TRG 4', 'KOPER', 'SI']</t>
   </si>
   <si>
+    <t>UNIVERZA NA PRIMORSKEM</t>
+  </si>
+  <si>
     <t>SK BANSKA01</t>
   </si>
   <si>
     <t>['NARODNA 12', 'BANSKA BYSTRICA', 'SK']</t>
   </si>
   <si>
+    <t>Univerzita Mateja Bela v Banskej Bystrici</t>
+  </si>
+  <si>
     <t>SK BRATISL02</t>
   </si>
   <si>
     <t>['SAFARIKOVO NAM 6', 'BRATISLAVA', 'SK']</t>
   </si>
   <si>
+    <t xml:space="preserve">UNIVERZITA KOMENSKEHO V BRATISLAVE                                                                                      </t>
+  </si>
+  <si>
     <t>SK PRESOV01</t>
   </si>
   <si>
     <t>['UL 17 NOVEMBRA 15', 'PRESOV', 'SK']</t>
   </si>
   <si>
+    <t>PRESOVSKÁ UNIVERZITA V PRESOVE</t>
+  </si>
+  <si>
     <t>SK RUZOMBE01</t>
   </si>
   <si>
     <t>['NAMESTIE ANDREJA HLINKU 60', 'RUZOMBEROK', 'SK']</t>
   </si>
   <si>
+    <t>KATOLÍCKA UNIVERZITA V RUZOMBERKU</t>
+  </si>
+  <si>
     <t>SK TRNAVA02</t>
   </si>
   <si>
     <t>['NAM J HERDU 2', 'TRNAVA', 'SK']</t>
   </si>
   <si>
+    <t>UNIVERZITA SV. CYRILA A METODA V TRNAVA</t>
+  </si>
+  <si>
     <t>TR ANTALYA01</t>
   </si>
   <si>
     <t>['DUMLUPINAR BULVARI  Kampus', 'ANTALYA', 'TR']</t>
   </si>
   <si>
+    <t>Akdeniz Üniversitesi</t>
+  </si>
+  <si>
     <t>TR ANTALYA04</t>
   </si>
   <si>
     <t>['Cikcilli Mahallesi  Saraybeleni Cad. No:7', 'Alanya', 'TR']</t>
   </si>
   <si>
+    <t>ALANYA HEP UNIVERSITY</t>
+  </si>
+  <si>
     <t>TR CANAKKA01</t>
   </si>
   <si>
     <t>['TERZIOGLU KAMPUSU REKTORLUK', 'CANAKKALE', 'TR']</t>
   </si>
   <si>
+    <t>Canakkale Onsekiz Mart Üniversitesi</t>
+  </si>
+  <si>
     <t>TR ESKISEH03</t>
   </si>
   <si>
     <t>['ESKISEHIR TEKNIK UNIVERSITESI REKTORLUGU IKI EYLUL TEPEBASI', 'ESKISEHIR', 'TR']</t>
   </si>
   <si>
+    <t>ESKISEHIR TEKNIK UNIVERSITESI</t>
+  </si>
+  <si>
     <t>TR IZMIR01</t>
   </si>
   <si>
     <t>['CUMHURIYET BULVARI  144', 'ALSANCAK IZMIR', 'TR']</t>
   </si>
   <si>
+    <t>Dokuz Eylül Üniversitesi, Izmir</t>
+  </si>
+  <si>
     <t>TR KARS01</t>
   </si>
   <si>
     <t>['PASACAYIRI', 'KARS', 'TR']</t>
   </si>
   <si>
+    <t>Kafkas Universitesi</t>
+  </si>
+  <si>
     <t>TR TRABZON04</t>
   </si>
   <si>
     <t>['Trabzon University, Fatih Education Faculty, F Block, First Floor, Office of International Relations, Akçaabat/TRABZON', 'TRABZON', 'TR']</t>
+  </si>
+  <si>
+    <t>TRABZON UNIVERSITY</t>
   </si>
 </sst>
 </file>
@@ -384,11 +543,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:B55" totalsRowShown="0">
-  <autoFilter ref="A1:B55"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:C55" totalsRowShown="0">
+  <autoFilter ref="A1:C55"/>
+  <tableColumns count="3">
     <tableColumn id="1" name="ERASMUS CODE" dataDxfId="0"/>
     <tableColumn id="2" name="Address" dataDxfId="0"/>
+    <tableColumn id="3" name="Univerzita" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,450 +839,615 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>64</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>67</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>70</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>73</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>76</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>79</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>85</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>88</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>94</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>100</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>103</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>106</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>109</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>112</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>115</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>118</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>124</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>127</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>130</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>133</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>136</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>145</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>98</v>
+        <v>147</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>148</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>151</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>154</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>105</v>
+        <v>157</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>